<commit_message>
Updated Piecharts and PCAs
</commit_message>
<xml_diff>
--- a/Structure_ClusterAssignMLGs_locPrior.xlsx
+++ b/Structure_ClusterAssignMLGs_locPrior.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wslch365-my.sharepoint.com/personal/lia_baumann_wsl_ch/Documents/R/truffles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{F26431A7-BDB7-4FAB-ADE6-B6DC0C796DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BABB1B2-C03A-4532-9446-8CE83ABE4A01}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{F26431A7-BDB7-4FAB-ADE6-B6DC0C796DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C6494D9-0178-4E40-B3AE-BBE9DEEDB87F}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{06436BD7-12A4-460A-BE0F-91FED5F87538}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{06436BD7-12A4-460A-BE0F-91FED5F87538}"/>
   </bookViews>
   <sheets>
     <sheet name="ClumppIndFileMLGref_locP_runLia" sheetId="1" r:id="rId1"/>
@@ -3393,10 +3393,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3757,9 +3753,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47902FC0-B533-4CED-AEC0-FE7F2C83BE72}">
   <dimension ref="A1:AA468"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:L1048576"/>
+      <selection pane="bottomLeft" activeCell="AB1" sqref="AB1:AF1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -42623,7 +42619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B25051-B2D6-4EEE-8F38-55950A1A9395}">
   <dimension ref="A1:C468"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>